<commit_message>
Ersatt "hårdkodade" värden under avsnitt 4
</commit_message>
<xml_diff>
--- a/Indata/ohalsotal.xlsx
+++ b/Indata/ohalsotal.xlsx
@@ -47,7 +47,7 @@
     <t xml:space="preserve">2024</t>
   </si>
   <si>
-    <t xml:space="preserve">10</t>
+    <t xml:space="preserve">11</t>
   </si>
   <si>
     <t xml:space="preserve">00 Riket</t>
@@ -65,7 +65,7 @@
     <t xml:space="preserve">Riket</t>
   </si>
   <si>
-    <t xml:space="preserve">oktober</t>
+    <t xml:space="preserve">november</t>
   </si>
   <si>
     <t xml:space="preserve">17 Värmlands län</t>
@@ -482,7 +482,7 @@
         <v>14</v>
       </c>
       <c r="G2" t="n">
-        <v>22.4</v>
+        <v>22.5</v>
       </c>
       <c r="H2" t="s">
         <v>15</v>
@@ -514,7 +514,7 @@
         <v>14</v>
       </c>
       <c r="G3" t="n">
-        <v>28.1</v>
+        <v>28.3</v>
       </c>
       <c r="H3" t="s">
         <v>19</v>
@@ -546,7 +546,7 @@
         <v>14</v>
       </c>
       <c r="G4" t="n">
-        <v>26.5</v>
+        <v>26.7</v>
       </c>
       <c r="H4" t="s">
         <v>22</v>
@@ -578,7 +578,7 @@
         <v>14</v>
       </c>
       <c r="G5" t="n">
-        <v>28</v>
+        <v>28.2</v>
       </c>
       <c r="H5" t="s">
         <v>25</v>
@@ -610,7 +610,7 @@
         <v>27</v>
       </c>
       <c r="G6" t="n">
-        <v>27</v>
+        <v>27.2</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -642,7 +642,7 @@
         <v>27</v>
       </c>
       <c r="G7" t="n">
-        <v>34.8</v>
+        <v>35.2</v>
       </c>
       <c r="H7" t="s">
         <v>19</v>
@@ -674,7 +674,7 @@
         <v>27</v>
       </c>
       <c r="G8" t="n">
-        <v>32.3</v>
+        <v>32.6</v>
       </c>
       <c r="H8" t="s">
         <v>22</v>
@@ -706,7 +706,7 @@
         <v>27</v>
       </c>
       <c r="G9" t="n">
-        <v>34.1</v>
+        <v>34.5</v>
       </c>
       <c r="H9" t="s">
         <v>25</v>
@@ -738,7 +738,7 @@
         <v>28</v>
       </c>
       <c r="G10" t="n">
-        <v>18</v>
+        <v>18.1</v>
       </c>
       <c r="H10" t="s">
         <v>15</v>
@@ -770,7 +770,7 @@
         <v>28</v>
       </c>
       <c r="G11" t="n">
-        <v>21.7</v>
+        <v>21.9</v>
       </c>
       <c r="H11" t="s">
         <v>19</v>
@@ -802,7 +802,7 @@
         <v>28</v>
       </c>
       <c r="G12" t="n">
-        <v>21.1</v>
+        <v>21.2</v>
       </c>
       <c r="H12" t="s">
         <v>22</v>
@@ -834,7 +834,7 @@
         <v>28</v>
       </c>
       <c r="G13" t="n">
-        <v>22.2</v>
+        <v>22.3</v>
       </c>
       <c r="H13" t="s">
         <v>25</v>

</xml_diff>